<commit_message>
All Clients running code
</commit_message>
<xml_diff>
--- a/i2o_SU_SanityBQTest/Testcases/testscenarios-cedar.xlsx
+++ b/i2o_SU_SanityBQTest/Testcases/testscenarios-cedar.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ankit-WorkArea-Automation\GithubProjects\GitWorkspace_SU\i2o_SU_SanityBQTest\Testcases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A60D2E50-0E66-4FF5-8178-9ED790DF4699}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13A52713-A99C-465C-9363-267A12D5E695}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="16560" windowHeight="8940" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Scenarios" sheetId="1" r:id="rId1"/>
     <sheet name="HompeageTest" sheetId="2" r:id="rId2"/>
     <sheet name="AsinLevelTest" sheetId="9" r:id="rId3"/>
+    <sheet name="HompeageTest (2)" sheetId="10" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -30,14 +31,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="79">
   <si>
     <t>Execution status</t>
   </si>
   <si>
-    <t>yes</t>
-  </si>
-  <si>
     <t>NO</t>
   </si>
   <si>
@@ -114,6 +112,12 @@
   </si>
   <si>
     <t>Asins</t>
+  </si>
+  <si>
+    <t>Validate COGS for TOP 5 Products in prestage and Data mart</t>
+  </si>
+  <si>
+    <t>Validate UNITS for TOP 5 Products in prestage and Data mart</t>
   </si>
   <si>
     <t>Sales Analysis</t>
@@ -167,18 +171,12 @@
     <t>20</t>
   </si>
   <si>
-    <t>Validate COGS for TOP 10 Products in prestage and Data mart</t>
-  </si>
-  <si>
-    <t>Validate UNITS for TOP 10 Products in prestage and Data mart</t>
+    <t>PRODUCT_UNITS</t>
   </si>
   <si>
     <t>PRODUCT_COGS</t>
   </si>
   <si>
-    <t>PRODUCT_UNITS</t>
-  </si>
-  <si>
     <t>LAST_WEEK_REVENUE</t>
   </si>
   <si>
@@ -188,7 +186,16 @@
     <t>LAST_WEEK_BBX_PCNT</t>
   </si>
   <si>
-    <t>05/22/2020 00:57:37</t>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>B01669UNR8</t>
+  </si>
+  <si>
+    <t>47244.75</t>
   </si>
   <si>
     <t>B0063A0NZI</t>
@@ -218,10 +225,7 @@
     <t>34980.0</t>
   </si>
   <si>
-    <t>31680.0</t>
-  </si>
-  <si>
-    <t>30214.34</t>
+    <t>104.0</t>
   </si>
   <si>
     <t>157.0</t>
@@ -239,43 +243,34 @@
     <t>316.0</t>
   </si>
   <si>
-    <t>287.0</t>
-  </si>
-  <si>
-    <t>78.0</t>
-  </si>
-  <si>
-    <t>Pass</t>
-  </si>
-  <si>
-    <t>05/22/2020 01:08:49</t>
+    <t>Week</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>05/29/2020 14:32:10</t>
+  </si>
+  <si>
+    <t>2020-05-17</t>
+  </si>
+  <si>
+    <t>142313.93000000002</t>
+  </si>
+  <si>
+    <t>895.0</t>
+  </si>
+  <si>
+    <t>95.30388888888889</t>
+  </si>
+  <si>
+    <t>95.3038888888889</t>
   </si>
   <si>
     <t>Fail</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
-    <t>05/22/2020 01:11:42</t>
-  </si>
-  <si>
-    <t>05/22/2020 01:11:43</t>
-  </si>
-  <si>
-    <t>B01669UNR8</t>
-  </si>
-  <si>
-    <t>30146.65</t>
-  </si>
-  <si>
-    <t>B07SZW8SH4</t>
-  </si>
-  <si>
-    <t>28350.0</t>
-  </si>
-  <si>
-    <t>25110.0</t>
+    <t>05/30/2020 00:11:32</t>
   </si>
 </sst>
 </file>
@@ -401,74 +396,43 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="26">
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="solid">
+  <dxfs count="39">
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
           <fgColor indexed="64"/>
           <bgColor theme="0"/>
         </patternFill>
@@ -478,7 +442,37 @@
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
       <fill>
-        <patternFill patternType="solid">
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
           <fgColor indexed="64"/>
           <bgColor theme="0"/>
         </patternFill>
@@ -488,23 +482,22 @@
     <dxf>
       <border outline="0">
         <top style="thin">
-          <color indexed="64"/>
+          <color rgb="FF000000"/>
         </top>
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
+      <fill>
+        <patternFill>
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFFFFFFF"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <border outline="0">
         <bottom style="thin">
-          <color indexed="64"/>
+          <color rgb="FF000000"/>
         </bottom>
       </border>
     </dxf>
@@ -545,6 +538,148 @@
       </border>
     </dxf>
     <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <fgColor indexed="64"/>
@@ -589,7 +724,7 @@
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
       <fill>
-        <patternFill patternType="solid">
+        <patternFill>
           <fgColor indexed="64"/>
           <bgColor theme="0"/>
         </patternFill>
@@ -707,36 +842,54 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{DD55D255-C2A8-4898-9757-794873DEE3B9}" name="Table2" displayName="Table2" ref="A1:I4" totalsRowShown="0" headerRowDxfId="25" dataDxfId="23" headerRowBorderDxfId="24" tableBorderDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{DD55D255-C2A8-4898-9757-794873DEE3B9}" name="Table2" displayName="Table2" ref="A1:I4" totalsRowShown="0" headerRowDxfId="38" dataDxfId="36" headerRowBorderDxfId="37" tableBorderDxfId="35">
   <autoFilter ref="A1:I4" xr:uid="{2CB686C0-B5D9-45FA-9C71-84AF96746E12}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{EFDA0D10-DAB9-4DB5-A509-C9E0D66B0934}" name="TestID" dataDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{A24E5DA9-698A-4F89-A18D-1EA81D723A79}" name="Module" dataDxfId="20"/>
-    <tableColumn id="3" xr3:uid="{38F23A6E-896D-494C-963B-91A84C3F4369}" name="Scenario Name " dataDxfId="19"/>
-    <tableColumn id="4" xr3:uid="{AACDA2AC-8595-4777-94BE-3C07FDF41F94}" name="TestData" dataDxfId="18"/>
-    <tableColumn id="5" xr3:uid="{CE46EF65-C67C-4C47-B43D-AC997478A487}" name="Columname" dataDxfId="17"/>
-    <tableColumn id="6" xr3:uid="{B6F42A65-D827-448F-AD7C-21D37629A529}" name="Prestage Value" dataDxfId="16"/>
-    <tableColumn id="7" xr3:uid="{5C04FBED-D8D1-41BD-B6FE-DEBA88FA22EC}" name="Mart Value" dataDxfId="15"/>
-    <tableColumn id="8" xr3:uid="{9628BC46-B7B8-4319-87FC-7736DF04D7A0}" name="Difference" dataDxfId="14"/>
-    <tableColumn id="9" xr3:uid="{51FA0C3F-3EEF-43DF-B81F-5EB125970849}" name="Status" dataDxfId="13"/>
+    <tableColumn id="1" xr3:uid="{EFDA0D10-DAB9-4DB5-A509-C9E0D66B0934}" name="TestID" dataDxfId="34"/>
+    <tableColumn id="2" xr3:uid="{A24E5DA9-698A-4F89-A18D-1EA81D723A79}" name="Module" dataDxfId="33"/>
+    <tableColumn id="3" xr3:uid="{38F23A6E-896D-494C-963B-91A84C3F4369}" name="Scenario Name " dataDxfId="32"/>
+    <tableColumn id="4" xr3:uid="{AACDA2AC-8595-4777-94BE-3C07FDF41F94}" name="TestData" dataDxfId="31"/>
+    <tableColumn id="5" xr3:uid="{CE46EF65-C67C-4C47-B43D-AC997478A487}" name="Week" dataDxfId="30"/>
+    <tableColumn id="6" xr3:uid="{B6F42A65-D827-448F-AD7C-21D37629A529}" name="Prestage Value" dataDxfId="29"/>
+    <tableColumn id="7" xr3:uid="{5C04FBED-D8D1-41BD-B6FE-DEBA88FA22EC}" name="Mart Value" dataDxfId="28"/>
+    <tableColumn id="8" xr3:uid="{9628BC46-B7B8-4319-87FC-7736DF04D7A0}" name="Difference" dataDxfId="27"/>
+    <tableColumn id="9" xr3:uid="{51FA0C3F-3EEF-43DF-B81F-5EB125970849}" name="Status" dataDxfId="26"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5D7EC7D3-B8C5-4CD6-B81E-DD605F1158F5}" name="Table1" displayName="Table1" ref="A1:I21" totalsRowShown="0" headerRowDxfId="12" dataDxfId="10" headerRowBorderDxfId="11" tableBorderDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5D7EC7D3-B8C5-4CD6-B81E-DD605F1158F5}" name="Table1" displayName="Table1" ref="A1:I21" totalsRowShown="0" headerRowDxfId="25" dataDxfId="23" headerRowBorderDxfId="24" tableBorderDxfId="22">
   <autoFilter ref="A1:I21" xr:uid="{58023CD7-9179-421F-8E4D-220C140C11FD}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{66655932-DF3E-4F71-9A38-2694283919F9}" name="TestID" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{C926FDE5-10D4-4479-BCAF-D48FE648A502}" name="Module" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{CAE470C0-BBD2-4432-971C-9297D3F81E96}" name="Scenario Name " dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{08081835-A686-49DA-BA21-C6870155F04C}" name="TestData" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{EF87C231-A92D-47C6-BC12-A67DCEA15C6B}" name="Asins" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{E1E79FBC-4C2A-4384-8CCE-FA4326B489F6}" name="Prestage Value" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{DE522374-8968-4FEB-8694-8FE43D09F13F}" name="Mart Value" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{86C8BBD2-1144-4CFF-9F3D-72FBBA7DA20B}" name="Difference" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{AFF141D2-C7D5-4326-9BA4-56B045AB3110}" name="Status" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{66655932-DF3E-4F71-9A38-2694283919F9}" name="TestID" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{C926FDE5-10D4-4479-BCAF-D48FE648A502}" name="Module" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{CAE470C0-BBD2-4432-971C-9297D3F81E96}" name="Scenario Name " dataDxfId="19"/>
+    <tableColumn id="4" xr3:uid="{08081835-A686-49DA-BA21-C6870155F04C}" name="TestData" dataDxfId="18"/>
+    <tableColumn id="5" xr3:uid="{EF87C231-A92D-47C6-BC12-A67DCEA15C6B}" name="Asins" dataDxfId="17"/>
+    <tableColumn id="6" xr3:uid="{E1E79FBC-4C2A-4384-8CCE-FA4326B489F6}" name="Prestage Value" dataDxfId="16"/>
+    <tableColumn id="7" xr3:uid="{DE522374-8968-4FEB-8694-8FE43D09F13F}" name="Mart Value" dataDxfId="15"/>
+    <tableColumn id="8" xr3:uid="{86C8BBD2-1144-4CFF-9F3D-72FBBA7DA20B}" name="Difference" dataDxfId="14"/>
+    <tableColumn id="9" xr3:uid="{AFF141D2-C7D5-4326-9BA4-56B045AB3110}" name="Status" dataDxfId="13"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{93129CC7-19C3-4EE7-AC55-E827F25CC549}" name="Table24" displayName="Table24" ref="A1:I4" totalsRowShown="0" headerRowDxfId="12" dataDxfId="10" headerRowBorderDxfId="11" tableBorderDxfId="9">
+  <autoFilter ref="A1:I4" xr:uid="{2CB686C0-B5D9-45FA-9C71-84AF96746E12}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{AC9C42F6-A11F-44EE-8703-52A9E0E55C95}" name="TestID" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{F11CC7E8-9444-4457-B565-F708B463EFD3}" name="Module" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{3F789C1B-B13D-407A-891F-CD571D470A14}" name="Scenario Name " dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{30C61746-3284-45F7-87EF-DACFD36DEA59}" name="TestData" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{548255C8-A389-403C-8124-AC74804BA137}" name="Columname" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{6441A740-6F44-4A2C-A0CF-2B22A45D21CA}" name="Prestage Value" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{FDE63777-F390-4663-88FA-101C174CB06D}" name="Mart Value" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{30EB1FA8-05B2-4674-A0AF-69192C805FA3}" name="Difference" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{525B0E89-F5E5-4873-9FA8-9894D8DDCDFB}" name="Status" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1065,8 +1218,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1078,52 +1231,49 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="C2" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
-        <v>75</v>
-      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4" s="8"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C5" s="8"/>
     </row>
@@ -1145,8 +1295,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1165,118 +1315,118 @@
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="F1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="H1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="7" t="s">
-        <v>12</v>
-      </c>
       <c r="I1" s="7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2">
-        <v>56142.98</v>
-      </c>
-      <c r="G2">
-        <v>104934.39</v>
+        <v>47</v>
+      </c>
+      <c r="E2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F2" t="s">
+        <v>73</v>
+      </c>
+      <c r="G2" t="s">
+        <v>73</v>
       </c>
       <c r="H2" t="n">
-        <v>-48791.409999999996</v>
+        <v>0.0</v>
       </c>
       <c r="I2" t="s">
-        <v>72</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3">
-        <v>210</v>
-      </c>
-      <c r="G3">
-        <v>584</v>
+        <v>48</v>
+      </c>
+      <c r="E3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F3" t="s">
+        <v>74</v>
+      </c>
+      <c r="G3" t="s">
+        <v>74</v>
       </c>
       <c r="H3" t="n">
-        <v>-374.0</v>
+        <v>0.0</v>
       </c>
       <c r="I3" t="s">
-        <v>72</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:9" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4">
-        <v>95.182203389830519</v>
-      </c>
-      <c r="G4">
-        <v>91.643939393939405</v>
+        <v>49</v>
+      </c>
+      <c r="E4" t="s">
+        <v>72</v>
+      </c>
+      <c r="F4" t="s">
+        <v>75</v>
+      </c>
+      <c r="G4" t="s">
+        <v>76</v>
       </c>
       <c r="H4" t="n">
-        <v>3.538263999999998</v>
+        <v>-1.4210854715202004E-14</v>
       </c>
       <c r="I4" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -1301,7 +1451,7 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="E2" sqref="E2:I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1320,42 +1470,42 @@
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="H1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="7" t="s">
-        <v>12</v>
-      </c>
       <c r="I1" s="7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>46</v>
@@ -1369,44 +1519,44 @@
       <c r="G2" t="s">
         <v>53</v>
       </c>
-      <c r="H2" t="n">
-        <v>0.0</v>
+      <c r="H2">
+        <v>0</v>
       </c>
       <c r="I2" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="2"/>
       <c r="E3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G3" t="s">
-        <v>55</v>
-      </c>
-      <c r="H3" t="n">
-        <v>0.0</v>
+        <v>53</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
       </c>
       <c r="I3" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="2"/>
@@ -1419,19 +1569,19 @@
       <c r="G4" t="s">
         <v>55</v>
       </c>
-      <c r="H4" t="n">
-        <v>0.0</v>
+      <c r="H4">
+        <v>0</v>
       </c>
       <c r="I4" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="2"/>
@@ -1444,19 +1594,19 @@
       <c r="G5" t="s">
         <v>57</v>
       </c>
-      <c r="H5" t="n">
-        <v>0.0</v>
+      <c r="H5">
+        <v>0</v>
       </c>
       <c r="I5" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="2"/>
@@ -1469,74 +1619,74 @@
       <c r="G6" t="s">
         <v>57</v>
       </c>
-      <c r="H6" t="n">
-        <v>0.0</v>
+      <c r="H6">
+        <v>0</v>
       </c>
       <c r="I6" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="2"/>
       <c r="E7" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="F7" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G7" t="s">
-        <v>58</v>
-      </c>
-      <c r="H7" t="n">
-        <v>0.0</v>
+        <v>59</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
       </c>
       <c r="I7" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="2"/>
       <c r="E8" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="F8" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G8" t="s">
-        <v>58</v>
-      </c>
-      <c r="H8" t="n">
-        <v>0.0</v>
+        <v>59</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
       </c>
       <c r="I8" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="2"/>
       <c r="E9" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F9" t="s">
         <v>60</v>
@@ -1544,49 +1694,49 @@
       <c r="G9" t="s">
         <v>60</v>
       </c>
-      <c r="H9" t="n">
-        <v>0.0</v>
+      <c r="H9">
+        <v>0</v>
       </c>
       <c r="I9" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="2"/>
       <c r="E10" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G10" t="s">
-        <v>61</v>
-      </c>
-      <c r="H10" t="n">
-        <v>0.0</v>
+        <v>60</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
       </c>
       <c r="I10" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="2"/>
       <c r="E11" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="F11" t="s">
         <v>62</v>
@@ -1594,25 +1744,25 @@
       <c r="G11" t="s">
         <v>62</v>
       </c>
-      <c r="H11" t="n">
-        <v>0.0</v>
+      <c r="H11">
+        <v>0</v>
       </c>
       <c r="I11" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C12" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>47</v>
       </c>
       <c r="E12" t="s">
         <v>52</v>
@@ -1623,44 +1773,44 @@
       <c r="G12" t="s">
         <v>63</v>
       </c>
-      <c r="H12" t="n">
-        <v>0.0</v>
+      <c r="H12">
+        <v>0</v>
       </c>
       <c r="I12" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="2"/>
       <c r="E13" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G13" t="s">
-        <v>64</v>
-      </c>
-      <c r="H13" t="n">
-        <v>0.0</v>
+        <v>63</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
       </c>
       <c r="I13" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="2"/>
@@ -1673,19 +1823,19 @@
       <c r="G14" t="s">
         <v>64</v>
       </c>
-      <c r="H14" t="n">
-        <v>0.0</v>
+      <c r="H14">
+        <v>0</v>
       </c>
       <c r="I14" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="2"/>
@@ -1698,19 +1848,19 @@
       <c r="G15" t="s">
         <v>65</v>
       </c>
-      <c r="H15" t="n">
-        <v>0.0</v>
+      <c r="H15">
+        <v>0</v>
       </c>
       <c r="I15" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="2"/>
@@ -1723,24 +1873,24 @@
       <c r="G16" t="s">
         <v>65</v>
       </c>
-      <c r="H16" t="n">
-        <v>0.0</v>
+      <c r="H16">
+        <v>0</v>
       </c>
       <c r="I16" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="2"/>
       <c r="E17" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="F17" t="s">
         <v>66</v>
@@ -1748,24 +1898,24 @@
       <c r="G17" t="s">
         <v>66</v>
       </c>
-      <c r="H17" t="n">
-        <v>0.0</v>
+      <c r="H17">
+        <v>0</v>
       </c>
       <c r="I17" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="2"/>
       <c r="E18" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="F18" t="s">
         <v>66</v>
@@ -1773,24 +1923,24 @@
       <c r="G18" t="s">
         <v>66</v>
       </c>
-      <c r="H18" t="n">
-        <v>0.0</v>
+      <c r="H18">
+        <v>0</v>
       </c>
       <c r="I18" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="2"/>
       <c r="E19" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F19" t="s">
         <v>67</v>
@@ -1798,61 +1948,61 @@
       <c r="G19" t="s">
         <v>67</v>
       </c>
-      <c r="H19" t="n">
-        <v>0.0</v>
+      <c r="H19">
+        <v>0</v>
       </c>
       <c r="I19" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="2"/>
       <c r="E20" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G20" t="s">
-        <v>68</v>
-      </c>
-      <c r="H20" t="n">
-        <v>0.0</v>
+        <v>67</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
       </c>
       <c r="I20" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="2"/>
       <c r="E21" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="F21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G21" t="s">
-        <v>69</v>
-      </c>
-      <c r="H21" t="n">
-        <v>0.0</v>
+        <v>68</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
       </c>
       <c r="I21" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1863,4 +2013,127 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D78E3C23-DCF4-491F-89DC-7A2317CA6637}">
+  <dimension ref="A1:I4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" style="4" width="8.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="4" width="13.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="4" width="57.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="4" width="28.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="4" width="13.85546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="4" width="20.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="4" width="19.28515625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="4" width="12.5703125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="4" width="9.85546875" collapsed="true"/>
+    <col min="10" max="16384" style="4" width="9.140625" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2"/>
+      <c r="G2"/>
+      <c r="H2"/>
+      <c r="I2"/>
+    </row>
+    <row r="3" spans="1:9" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3"/>
+      <c r="G3"/>
+      <c r="H3"/>
+      <c r="I3"/>
+    </row>
+    <row r="4" spans="1:9" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4"/>
+      <c r="G4"/>
+      <c r="H4"/>
+      <c r="I4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup fitToWidth="0" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>